<commit_message>
Names on leaderboard are all functioning well
</commit_message>
<xml_diff>
--- a/transponder_names.xlsx
+++ b/transponder_names.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Jesus</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Danielle</t>
+          <t>Brian</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Kari</t>
+          <t>Mark</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Emily</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Brandon</t>
+          <t>David</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Charles</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Makayla</t>
+          <t>Megan</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Brenda</t>
+          <t>Maria</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Andrew</t>
+          <t>Charles</t>
         </is>
       </c>
     </row>
@@ -561,43 +561,43 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Jessica</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RZ10761</t>
+          <t>CS34132</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Tracey</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CS34132</t>
+          <t>CR48188</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Whitney</t>
+          <t>Andrea</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CR48188</t>
+          <t>RZ10761</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Tyler</t>
+          <t>Heather</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Jason</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Christian</t>
+          <t>Michael</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Tyler</t>
         </is>
       </c>
     </row>
@@ -645,367 +645,331 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Kirk</t>
+          <t>Amanda</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CX19285</t>
+          <t>RZ43503</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>James</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PF79070</t>
+          <t>LZ73964</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Kristin</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>RF48933</t>
+          <t>KP55121</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Erica</t>
+          <t>Lisa</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RZ02081</t>
+          <t>CW09719</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Andre</t>
+          <t>Michelle</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RR18114</t>
+          <t>SF04172</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Alexandra</t>
+          <t>Joshua</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>RZ39892</t>
+          <t>RR10973</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>James</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>RX72266</t>
+          <t>HH54287</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Todd</t>
+          <t>Patricia</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>LR40395</t>
+          <t>RR18114</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Kelly</t>
+          <t>Debbie</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LZ73964</t>
+          <t>KP31430</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Kathleen</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>RZ43503</t>
+          <t>PF79070</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>Brandy</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>RR10973</t>
+          <t>RF48933</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Isabel</t>
+          <t>Debbie</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CW09719</t>
+          <t>LR40395</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Debra</t>
+          <t>Shane</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SC75193</t>
+          <t>RZ02081</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kelly</t>
+          <t>Robert</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>HH54287</t>
+          <t>GK67167</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Eric</t>
+          <t>George</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>KP31430</t>
+          <t>CX19285</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Mason</t>
+          <t>Tracie</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SF04172</t>
+          <t>SC75193</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Stacy</t>
+          <t>Christopher</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>KP55121</t>
+          <t>RZ39892</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Tracey</t>
+          <t>Richard</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GK67167</t>
+          <t>RX72266</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Evelyn</t>
+          <t>Victor</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>VG76471</t>
+          <t>FW08700</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>Kevin</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>KR51169</t>
+          <t>VG76471</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tony</t>
+          <t>Cody</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>FW08700</t>
+          <t>KR51169</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Chad</t>
+          <t>William</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>RZ41573</t>
+          <t>NK39779</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Douglas</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>NK39779</t>
+          <t>RZ41573</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Jennifer</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>SC75193</t>
+          <t>RX45371</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sylvia</t>
+          <t>Lisa</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>RX45371</t>
+          <t>SC90979</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Tara</t>
+          <t>Timothy</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SC90979</t>
+          <t>GZ52385</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>Sean</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GZ52385</t>
+          <t>SF17035</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>David</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>SF17035</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Mike</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>KL02453</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Kyle</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>SC89480</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Rachel</t>
+          <t>Catherine</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
initial commit on branch deployment
</commit_message>
<xml_diff>
--- a/transponder_names.xlsx
+++ b/transponder_names.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -973,6 +973,1038 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CC16014</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Charles</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CS75905</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Brandy</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CT28904</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Tammie</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CT87815</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Grant</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CT92889</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Charles</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CT96975</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Amy</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CX12515</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Roy</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CX49214</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Jeffrey</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>FF79131</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Justin</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>FN45797</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Karen</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>FV24748</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Autumn</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GF09766</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Walter</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GG14690</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Devon</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>GR26216</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GW62048</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>GX39059</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Mark</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>HC00233</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>HL04378</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Lance</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>HL50250</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Alexander</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>HN13964</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>HS58961</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Erik</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>HT59273</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>HW01751</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Tammy</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>HW50253</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Jesse</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>HW65477</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>HX16467</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Edward</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>HX21357</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>HZ41945</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Kristen</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>HZ96035</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>KF34985</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Richard</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>KS34599</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Christopher</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>KS47739</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Carly</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>KS56856</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Margaret</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>KW24617</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Dylan</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>LG28256</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Nicole</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>LK78228</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Lynn</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>LK78317</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Dominique</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>LS87752</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Wendy</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>LT24518</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Kent</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>LZ00982</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>NF50295</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Larry</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>NL08606</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Derrick</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>NN03951</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Susan</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>NP45921</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Andrea</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>NR49073</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>NS41086</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Sergio</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>PH79943</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>PH81273</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>William</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>PP73332</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>PR96113</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>PW09136</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Pamela</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>PZ34569</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Vincent</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>RK07262</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Duane</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>RP54841</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Tammy</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>RR12260</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>RR16125</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>RR52678</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>RR53564</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Dawn</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>RR60662</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Ashlee</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>RR62459</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Frank</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>RS08357</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Ricky</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>RW64613</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Rachel</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>RX39522</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Cathy</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>RX45668</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Scott</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>RX46250</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>RX46307</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>RX74391</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Cassandra</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>RX79269</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Suzanne</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>RX82727</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>RX94786</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Julie</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>RZ08899</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Robin</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>RZ25025</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>RZ42212</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Laurie</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>SC73747</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Joel</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>SC87824</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>SC89480</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Amy</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>SC89632</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>SF25765</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Patricia</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>SF27513</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>SZ88337</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Megan</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>TP10652</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>TR45652</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Jon</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>TV24571</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>VF36699</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Melissa</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>9992</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Allison</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>SK16113</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Vanessa</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add function that deletes the contents of metingen when app.py is run
</commit_message>
<xml_diff>
--- a/transponder_names.xlsx
+++ b/transponder_names.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -973,6 +973,1014 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CC16014</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Jacob</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CS75905</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Kelsey</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CT28904</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Kristina</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CT87815</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Kristi</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CT92889</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Brittney</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CT96975</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Joshua</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CX12515</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CX49214</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Teresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>FF79131</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Jordan</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>FN45797</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Karen</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>FV24748</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Jim</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GF09766</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Timothy</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GG14690</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Corey</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>GR26216</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Morgan</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GW62048</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>William</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>GX39059</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Richard</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>HC00233</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Carly</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>HL04378</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Susan</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>HL50250</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>HN13964</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>HS58961</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Alexander</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>HT59273</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Andrew</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>HW01751</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Jennifer</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>HW50253</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Cynthia</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>HW65477</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Elizabeth</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>HX16467</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>HX21357</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Kathryn</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>HZ41945</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Sara</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>HZ96035</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Melissa</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>KF34985</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Ryan</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>KS34599</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>KS47739</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Andrew</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>KS56856</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Melissa</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>KW24617</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>LG28256</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>LK78228</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Samantha</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>LK78317</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>LS87752</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Kathy</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>LT24518</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Kimberly</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>LZ00982</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Richard</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>NF50295</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Matthew</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>NL08606</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>NN03951</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Frank</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>NP45921</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>NR49073</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>NS41086</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Deanna</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>PH79943</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>PH81273</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Danielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>PP73332</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Theresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>PR96113</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>PW09136</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Erica</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>PZ34569</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Douglas</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>RK07262</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>RP54841</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>RR12260</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Amanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>RR16125</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Kylie</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>RR52678</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Joshua</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>RR53564</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Michele</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>RR60662</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Michele</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>RR62459</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Frances</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>RS08357</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>RW64613</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>RX39522</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Ryan</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>RX45668</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Patricia</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>RX46250</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Susan</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>RX46307</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Tyler</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>RX74391</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Janet</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>RX79269</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Philip</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>RX82727</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Barbara</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>RX94786</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>RZ08899</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Debra</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>RZ25025</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Cameron</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>RZ42212</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Tricia</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>SC73747</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Elizabeth</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>SC87824</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Kimberly</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>SC89480</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>SC89632</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Laura</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>SF25765</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Douglas</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>SZ88337</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>TP10652</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Lauren</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>TV24571</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Jennifer</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>VF36699</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Casey</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>9992</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Cameron</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>SK16113</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Matthew</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updates to todo.md and some slight changes
</commit_message>
<xml_diff>
--- a/transponder_names.xlsx
+++ b/transponder_names.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -973,6 +973,1014 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CC16014</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Ryan</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CS75905</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Melinda</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CT28904</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Nicole</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CT87815</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Michelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CT92889</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CT96975</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Tasha</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CX12515</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Randy</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CX49214</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>FF79131</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Renee</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>FN45797</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Sonya</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>FV24748</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Kenneth</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GF09766</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GG14690</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Brittany</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>GR26216</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Kristen</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GW62048</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Donald</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>GX39059</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Jonathan</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>HC00233</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Raymond</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>HL04378</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>HL50250</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Russell</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>HN13964</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>HS58961</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Tina</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>HT59273</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>HW01751</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Pamela</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>HW50253</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Cindy</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>HW65477</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Christine</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>HX16467</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Bryan</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>HX21357</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>HZ41945</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>HZ96035</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Amanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>KF34985</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Julie</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>KS34599</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Alexis</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>KS47739</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Lydia</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>KS56856</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Vicki</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>KW24617</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Samantha</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>LG28256</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Kristin</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>LK78228</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>William</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>LK78317</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Rhonda</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>LS87752</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Kathryn</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>LT24518</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Danielle</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>LZ00982</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Timothy</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>NF50295</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>NL08606</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Carmen</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>NN03951</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Keith</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>NP45921</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>NR49073</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Robin</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>NS41086</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Kathleen</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>PH79943</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>PH81273</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Matthew</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>PP73332</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>PR96113</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>PW09136</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Erika</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>PZ34569</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Tom</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>RK07262</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Stephen</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>RP54841</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Patricia</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>RR12260</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Hannah</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>RR16125</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Jacob</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>RR52678</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Bradley</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>RR53564</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Holly</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>RR60662</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Shannon</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>RR62459</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>RS08357</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Audrey</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>RW64613</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Michelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>RX39522</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>RX45668</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Matthew</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>RX46250</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Denise</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>RX46307</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Hector</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>RX74391</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Brittany</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>RX79269</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Matthew</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>RX82727</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Tracey</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>RX94786</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Michelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>RZ08899</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>RZ25025</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Elizabeth</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>RZ42212</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Kaitlyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>SC73747</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Dave</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>SC87824</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Debbie</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>SC89480</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Heather</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>SC89632</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>SF25765</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Wayne</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>SZ88337</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>TP10652</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>TV24571</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>VF36699</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Jeffrey</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>SK16113</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Julia</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>9992</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Brenda</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>